<commit_message>
Day 2: Added manual test cases for OrangeHRM login functionality
</commit_message>
<xml_diff>
--- a/manual-test-cases/login-test-cases.xlsx
+++ b/manual-test-cases/login-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAM\Documents\TestingProjects\login-functionality-testing\manual-test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C630EB-21E6-4301-834E-4374A97D87DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269001EC-50C3-4AA1-BC0B-3533227CC1A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
   <si>
     <t>Test_Case_Title</t>
   </si>
@@ -118,6 +118,198 @@
   </si>
   <si>
     <t>TC_020</t>
+  </si>
+  <si>
+    <t>Username: Admin  Paswword :admin123</t>
+  </si>
+  <si>
+    <t>User should get logged into its account successfully</t>
+  </si>
+  <si>
+    <t>User gets logged in  into his account</t>
+  </si>
+  <si>
+    <t>Verified</t>
+  </si>
+  <si>
+    <t>Login with invalid username and password</t>
+  </si>
+  <si>
+    <t>User on OragneHRM demo login page</t>
+  </si>
+  <si>
+    <t>1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter invalid username                       4. Enter valid password                       5. Click Login button</t>
+  </si>
+  <si>
+    <t>Username: any        Password:admin123</t>
+  </si>
+  <si>
+    <t>User should get an error message of Invalid Username</t>
+  </si>
+  <si>
+    <t>User gets a error message of invalid credentials</t>
+  </si>
+  <si>
+    <t>Login with valid username and invalid password</t>
+  </si>
+  <si>
+    <t>1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter valid username                       4. Enter invalid password                       5. Click Login button</t>
+  </si>
+  <si>
+    <t>User should get error message of invalid Input details</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>Login with invalid username and invalid password</t>
+  </si>
+  <si>
+    <t>1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter invalid username                       4. Enter invalid password                       5. Click Login button</t>
+  </si>
+  <si>
+    <t>Login with blank username and blank password</t>
+  </si>
+  <si>
+    <t>1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter blank username                       4. Enter blank password                       5. Click Login button</t>
+  </si>
+  <si>
+    <t>Username:       Password :</t>
+  </si>
+  <si>
+    <t>Username: Admin1 Password :admin23</t>
+  </si>
+  <si>
+    <t>Username: Admin  Password :admin23</t>
+  </si>
+  <si>
+    <t>User should get asked for input in username field and passwword field</t>
+  </si>
+  <si>
+    <t>The required input area is highlightened re and input required is showned.</t>
+  </si>
+  <si>
+    <t>Verify error message for invalid login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify password field is masked </t>
+  </si>
+  <si>
+    <t>Verify login button is clickable</t>
+  </si>
+  <si>
+    <t>Verify required field validation messages</t>
+  </si>
+  <si>
+    <t>1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter any username                       4. Enter any password                       5. Click Login button</t>
+  </si>
+  <si>
+    <t>Username:  12a     Password :asd8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Browser                                      2. Navigate to OrangeHRM login page                                                                              3.  Enter blank password                       </t>
+  </si>
+  <si>
+    <t>Paswword : any</t>
+  </si>
+  <si>
+    <t>The password entered in passwword field textbox should get masked</t>
+  </si>
+  <si>
+    <t>The password entered in passwword field textbox is masked</t>
+  </si>
+  <si>
+    <t>1. Open Browser                                      2. Navigate to OrangeHRM login page                                                                              3. Click Login button</t>
+  </si>
+  <si>
+    <t>****</t>
+  </si>
+  <si>
+    <t>The Login button should be clicakble(enabled) even without inputs</t>
+  </si>
+  <si>
+    <t>The Login button is clickable(enabled</t>
+  </si>
+  <si>
+    <t>Verify logout functionality after successful login</t>
+  </si>
+  <si>
+    <t>User on logged OragneHRM demo account page</t>
+  </si>
+  <si>
+    <t>1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter valid username                       4. Enter valid password                       5. Click Login button 6. click on logout button</t>
+  </si>
+  <si>
+    <t>User should be easily be able to log out of its respective account</t>
+  </si>
+  <si>
+    <t>User is being easily  able to log out of its respective account</t>
+  </si>
+  <si>
+    <t>Verify usrname conditions</t>
+  </si>
+  <si>
+    <t>a pop up  of valid input of(Input required) should appear until any input is given other than space</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Verify password conitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter any username                       4. Enter spaces as password                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter Spaces as username                       4. Enter valid password                      </t>
+  </si>
+  <si>
+    <t>Username: any      Password : spaces</t>
+  </si>
+  <si>
+    <t>Username: spaces Password : any</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A pop up (required) below username input field is shown  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A pop up (required) below Password input field is shown  </t>
+  </si>
+  <si>
+    <t>Case Sensitivity Check on Both</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter any casesensitive as username                       4. Enter casesensitive as password                        </t>
+  </si>
+  <si>
+    <t>Username: ADMIN        Password: ADMIN123</t>
+  </si>
+  <si>
+    <t>Multiple failed login</t>
+  </si>
+  <si>
+    <t>Username: any      Password : any</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter any casesensitive as username                       4. Enter casesensitive as password                     .5. Attempt login multiple times                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">User gets a error message of invalid credentials </t>
+  </si>
+  <si>
+    <t>User should get error message of invalid Input details until correct credentials are given</t>
+  </si>
+  <si>
+    <t>Verify page refresh after entering credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Browser                                      2. Navigate to OrangeHRM login page                                                            3. Enter any casesensitive as username                       4. Enter casesensitive as password                     .5. Click refresh button            </t>
+  </si>
+  <si>
+    <t>The input given should not reappear in the input field</t>
+  </si>
+  <si>
+    <t>The input given befeore refreshing gets removed from the input fields</t>
   </si>
 </sst>
 </file>
@@ -450,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +651,7 @@
     <col min="1" max="1" width="14.28515625" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
@@ -504,192 +696,396 @@
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="150" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -759,5 +1155,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Day 2: Added manual test casesfor OrangeHRM login Functionality
</commit_message>
<xml_diff>
--- a/manual-test-cases/login-test-cases.xlsx
+++ b/manual-test-cases/login-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAM\Documents\TestingProjects\login-functionality-testing\manual-test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269001EC-50C3-4AA1-BC0B-3533227CC1A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59492B95-D8D6-46E1-B173-09813DF5F822}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="E15" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>